<commit_message>
changed the code. its working now.
</commit_message>
<xml_diff>
--- a/trades.xlsx
+++ b/trades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e765c67e5fd66cdb/Desktop/stocks/profit loss calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{34F3568A-AB30-4D52-8EAC-5C2531301BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1448AEB1-FD79-43A7-81CC-22AB5FB865E3}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{34F3568A-AB30-4D52-8EAC-5C2531301BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D0EACA3-3DB8-4F02-9BFA-92CA45970ECD}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="340" windowWidth="10350" windowHeight="9570" xr2:uid="{068B3D48-7628-4D59-AA9C-41A2A16CDD8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{068B3D48-7628-4D59-AA9C-41A2A16CDD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Sell Price</t>
   </si>
@@ -72,6 +72,30 @@
   </si>
   <si>
     <t>Stock name</t>
+  </si>
+  <si>
+    <t>GDHG</t>
+  </si>
+  <si>
+    <t>LPTV</t>
+  </si>
+  <si>
+    <t>SNTI</t>
+  </si>
+  <si>
+    <t>LUCY</t>
+  </si>
+  <si>
+    <t>GOVX</t>
+  </si>
+  <si>
+    <t>OPTT</t>
+  </si>
+  <si>
+    <t>MBIO</t>
+  </si>
+  <si>
+    <t>ANVS</t>
   </si>
 </sst>
 </file>
@@ -133,10 +157,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D097AA50-67EC-425A-9287-BEDAFD0E2177}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -490,117 +510,287 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
-        <v>45476</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>45474</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>5.94</v>
+        <v>0.1895</v>
       </c>
       <c r="D2" s="1">
-        <v>6.35</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
-        <v>45476</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>45474</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1">
-        <v>3.15</v>
+        <v>0.15060000000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>2.69</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
-        <v>45476</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>45474</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="1">
-        <v>0.2165</v>
+        <v>0.48509999999999998</v>
       </c>
       <c r="D4" s="1">
-        <v>0.20599999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="E4" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
+        <v>45474</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="E5" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>45474</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.51649999999999996</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.49209999999999998</v>
+      </c>
+      <c r="E6" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>45474</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.61</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="E7" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>210.82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>226.46</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.47</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10.71</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
         <v>45476</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.94</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="E12" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>45476</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>45476</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.2165</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2">
+        <v>45476</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
         <v>2.8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D15" s="1">
         <v>2.2799999999999998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E15" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2">
         <v>45476</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C16" s="1">
         <v>4.79</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D16" s="1">
         <v>4.67</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E16" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2">
         <v>45476</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C17" s="1">
         <v>247.19</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2">
         <v>45476</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C18" s="1">
         <v>2.93</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D18" s="1">
         <v>3.15</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E18" s="1">
         <v>156</v>
       </c>
     </row>

</xml_diff>